<commit_message>
Survey resultsv part 1.
</commit_message>
<xml_diff>
--- a/Definition/Tables/Principles_classification/Summary.xlsx
+++ b/Definition/Tables/Principles_classification/Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clepore\Downloads\SSI_principles\Definition\Tables\Principles_classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53208089-2D28-41E4-B04A-84C778CDD458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3562037-08B5-4218-85A0-90AFB5EFD75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" activeTab="2" xr2:uid="{2F691BE0-650C-425B-994B-C0A8894E19E9}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10530" activeTab="3" xr2:uid="{2F691BE0-650C-425B-994B-C0A8894E19E9}"/>
   </bookViews>
   <sheets>
     <sheet name="SSI Principles" sheetId="1" r:id="rId1"/>
@@ -174,7 +174,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,6 +241,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="23">
     <border>
@@ -536,7 +548,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -618,6 +630,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -955,7 +979,7 @@
   <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1546,7 +1570,7 @@
   <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2126,7 +2150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D0380F8-8EF8-42F0-AD92-418BE1EF637C}">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -2710,8 +2734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFBFBA6-4E43-42FC-BA9D-A1ED5385B14C}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView zoomScale="93" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -2771,17 +2795,17 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="9"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="73">
+      <c r="D2" s="81">
         <v>6</v>
       </c>
-      <c r="E2" s="74">
+      <c r="E2" s="81">
         <v>7</v>
       </c>
       <c r="F2" s="74">
@@ -2812,15 +2836,15 @@
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="73">
+      <c r="B3" s="26"/>
+      <c r="C3" s="81">
         <v>6</v>
       </c>
       <c r="D3" s="72"/>
-      <c r="E3" s="75">
+      <c r="E3" s="81">
         <v>6</v>
       </c>
       <c r="F3" s="75"/>
@@ -2851,14 +2875,14 @@
       </c>
     </row>
     <row r="4" spans="1:17" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="73">
+      <c r="B4" s="26"/>
+      <c r="C4" s="81">
         <v>7</v>
       </c>
-      <c r="D4" s="73">
+      <c r="D4" s="81">
         <v>6</v>
       </c>
       <c r="E4" s="72"/>
@@ -2866,45 +2890,67 @@
       <c r="G4" s="74">
         <v>2</v>
       </c>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
+      <c r="H4" s="74">
+        <v>4</v>
+      </c>
+      <c r="I4" s="74">
+        <v>3</v>
+      </c>
       <c r="J4" s="73"/>
       <c r="K4" s="74"/>
       <c r="L4" s="74"/>
       <c r="M4" s="74"/>
       <c r="N4" s="74"/>
-      <c r="O4" s="74"/>
+      <c r="O4" s="74">
+        <v>2</v>
+      </c>
       <c r="P4" s="74"/>
-      <c r="Q4" s="74"/>
+      <c r="Q4" s="74">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:17" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="83"/>
       <c r="C5" s="79">
         <v>1</v>
       </c>
       <c r="D5" s="75"/>
       <c r="E5" s="76"/>
       <c r="F5" s="72"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="76"/>
+      <c r="G5" s="86">
+        <v>6</v>
+      </c>
+      <c r="H5" s="86">
+        <v>5</v>
+      </c>
+      <c r="I5" s="75">
+        <v>2</v>
+      </c>
+      <c r="J5" s="75">
+        <v>1</v>
+      </c>
+      <c r="K5" s="75">
+        <v>1</v>
+      </c>
+      <c r="L5" s="76">
+        <v>1</v>
+      </c>
       <c r="M5" s="76"/>
       <c r="N5" s="76"/>
       <c r="O5" s="75"/>
-      <c r="P5" s="75"/>
+      <c r="P5" s="75">
+        <v>2</v>
+      </c>
       <c r="Q5" s="75"/>
     </row>
     <row r="6" spans="1:17" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="B6" s="85"/>
       <c r="C6" s="73">
         <v>3</v>
       </c>
@@ -2914,43 +2960,83 @@
       <c r="E6" s="73">
         <v>2</v>
       </c>
-      <c r="F6" s="74"/>
+      <c r="F6" s="86">
+        <v>6</v>
+      </c>
       <c r="G6" s="72"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="74"/>
-      <c r="L6" s="74"/>
-      <c r="M6" s="74"/>
-      <c r="N6" s="74"/>
-      <c r="O6" s="74"/>
-      <c r="P6" s="74"/>
+      <c r="H6" s="86">
+        <v>7</v>
+      </c>
+      <c r="I6" s="74">
+        <v>3</v>
+      </c>
+      <c r="J6" s="74">
+        <v>2</v>
+      </c>
+      <c r="K6" s="74">
+        <v>2</v>
+      </c>
+      <c r="L6" s="74">
+        <v>1</v>
+      </c>
+      <c r="M6" s="74">
+        <v>1</v>
+      </c>
+      <c r="N6" s="74">
+        <v>1</v>
+      </c>
+      <c r="O6" s="74">
+        <v>2</v>
+      </c>
+      <c r="P6" s="74">
+        <v>2</v>
+      </c>
       <c r="Q6" s="74"/>
     </row>
     <row r="7" spans="1:17" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="85"/>
       <c r="C7" s="79">
         <v>4</v>
       </c>
       <c r="D7" s="75">
         <v>4</v>
       </c>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
+      <c r="E7" s="75">
+        <v>4</v>
+      </c>
+      <c r="F7" s="86">
+        <v>5</v>
+      </c>
+      <c r="G7" s="86">
+        <v>7</v>
+      </c>
       <c r="H7" s="72"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
-      <c r="L7" s="75"/>
+      <c r="I7" s="75">
+        <v>3</v>
+      </c>
+      <c r="J7" s="75">
+        <v>1</v>
+      </c>
+      <c r="K7" s="75">
+        <v>2</v>
+      </c>
+      <c r="L7" s="75">
+        <v>1</v>
+      </c>
       <c r="M7" s="75"/>
       <c r="N7" s="75"/>
-      <c r="O7" s="75"/>
-      <c r="P7" s="75"/>
-      <c r="Q7" s="75"/>
+      <c r="O7" s="75">
+        <v>2</v>
+      </c>
+      <c r="P7" s="75">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="75">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:17" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
       <c r="A8" s="3" t="s">
@@ -2963,46 +3049,88 @@
       <c r="D8" s="74">
         <v>4</v>
       </c>
-      <c r="E8" s="74"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="74"/>
-      <c r="H8" s="73"/>
+      <c r="E8" s="74">
+        <v>3</v>
+      </c>
+      <c r="F8" s="73">
+        <v>2</v>
+      </c>
+      <c r="G8" s="74">
+        <v>3</v>
+      </c>
+      <c r="H8" s="73">
+        <v>3</v>
+      </c>
       <c r="I8" s="72"/>
-      <c r="J8" s="74"/>
-      <c r="K8" s="74"/>
-      <c r="L8" s="74"/>
-      <c r="M8" s="74"/>
+      <c r="J8" s="74">
+        <v>5</v>
+      </c>
+      <c r="K8" s="74">
+        <v>2</v>
+      </c>
+      <c r="L8" s="74">
+        <v>4</v>
+      </c>
+      <c r="M8" s="74">
+        <v>1</v>
+      </c>
       <c r="N8" s="74"/>
-      <c r="O8" s="74"/>
-      <c r="P8" s="74"/>
-      <c r="Q8" s="74"/>
+      <c r="O8" s="74">
+        <v>2</v>
+      </c>
+      <c r="P8" s="74">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="74">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:17" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="10"/>
+      <c r="A9" s="87" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="88"/>
       <c r="C9" s="79"/>
       <c r="D9" s="75"/>
       <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
+      <c r="F9" s="75">
+        <v>1</v>
+      </c>
+      <c r="G9" s="75">
+        <v>2</v>
+      </c>
+      <c r="H9" s="75">
+        <v>1</v>
+      </c>
+      <c r="I9" s="75">
+        <v>5</v>
+      </c>
       <c r="J9" s="72"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="M9" s="75"/>
-      <c r="N9" s="75"/>
+      <c r="K9" s="91">
+        <v>4</v>
+      </c>
+      <c r="L9" s="91">
+        <v>6</v>
+      </c>
+      <c r="M9" s="91">
+        <v>4</v>
+      </c>
+      <c r="N9" s="91">
+        <v>4</v>
+      </c>
       <c r="O9" s="75"/>
-      <c r="P9" s="75"/>
-      <c r="Q9" s="75"/>
+      <c r="P9" s="75">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="75">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:17" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="10"/>
+      <c r="A10" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="88"/>
       <c r="C10" s="80">
         <v>1</v>
       </c>
@@ -3010,155 +3138,255 @@
         <v>2</v>
       </c>
       <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
+      <c r="F10" s="74">
+        <v>1</v>
+      </c>
+      <c r="G10" s="74">
+        <v>2</v>
+      </c>
+      <c r="H10" s="74">
+        <v>2</v>
+      </c>
+      <c r="I10" s="74">
+        <v>2</v>
+      </c>
+      <c r="J10" s="91">
+        <v>4</v>
+      </c>
       <c r="K10" s="72"/>
-      <c r="L10" s="74"/>
-      <c r="M10" s="74"/>
-      <c r="N10" s="74"/>
-      <c r="O10" s="74"/>
+      <c r="L10" s="91">
+        <v>8</v>
+      </c>
+      <c r="M10" s="91">
+        <v>2</v>
+      </c>
+      <c r="N10" s="91">
+        <v>3</v>
+      </c>
+      <c r="O10" s="74">
+        <v>1</v>
+      </c>
       <c r="P10" s="74"/>
       <c r="Q10" s="74"/>
     </row>
     <row r="11" spans="1:17" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="10"/>
+      <c r="B11" s="88"/>
       <c r="C11" s="79"/>
       <c r="D11" s="75">
         <v>1</v>
       </c>
       <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
+      <c r="F11" s="75">
+        <v>1</v>
+      </c>
+      <c r="G11" s="75">
+        <v>1</v>
+      </c>
+      <c r="H11" s="75">
+        <v>1</v>
+      </c>
+      <c r="I11" s="75">
+        <v>4</v>
+      </c>
+      <c r="J11" s="91">
+        <v>6</v>
+      </c>
+      <c r="K11" s="91">
+        <v>8</v>
+      </c>
       <c r="L11" s="72"/>
-      <c r="M11" s="75"/>
-      <c r="N11" s="75"/>
-      <c r="O11" s="75"/>
+      <c r="M11" s="91">
+        <v>2</v>
+      </c>
+      <c r="N11" s="91">
+        <v>3</v>
+      </c>
+      <c r="O11" s="75">
+        <v>1</v>
+      </c>
       <c r="P11" s="75"/>
-      <c r="Q11" s="75"/>
+      <c r="Q11" s="75">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:17" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="90"/>
       <c r="C12" s="80"/>
       <c r="D12" s="74"/>
       <c r="E12" s="74"/>
       <c r="F12" s="74"/>
-      <c r="G12" s="74"/>
+      <c r="G12" s="74">
+        <v>1</v>
+      </c>
       <c r="H12" s="74"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="74"/>
-      <c r="K12" s="74"/>
-      <c r="L12" s="74"/>
+      <c r="I12" s="74">
+        <v>1</v>
+      </c>
+      <c r="J12" s="91">
+        <v>4</v>
+      </c>
+      <c r="K12" s="91">
+        <v>2</v>
+      </c>
+      <c r="L12" s="91">
+        <v>2</v>
+      </c>
       <c r="M12" s="72"/>
-      <c r="N12" s="74"/>
-      <c r="O12" s="74"/>
+      <c r="N12" s="91">
+        <v>4</v>
+      </c>
+      <c r="O12" s="74">
+        <v>1</v>
+      </c>
       <c r="P12" s="74"/>
       <c r="Q12" s="74"/>
     </row>
     <row r="13" spans="1:17" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="10"/>
+      <c r="B13" s="88"/>
       <c r="C13" s="79"/>
       <c r="D13" s="75"/>
       <c r="E13" s="75"/>
       <c r="F13" s="75"/>
-      <c r="G13" s="75"/>
+      <c r="G13" s="75">
+        <v>1</v>
+      </c>
       <c r="H13" s="75"/>
       <c r="I13" s="75"/>
-      <c r="J13" s="75"/>
-      <c r="K13" s="75"/>
-      <c r="L13" s="75"/>
-      <c r="M13" s="75"/>
+      <c r="J13" s="91">
+        <v>4</v>
+      </c>
+      <c r="K13" s="91">
+        <v>3</v>
+      </c>
+      <c r="L13" s="91">
+        <v>3</v>
+      </c>
+      <c r="M13" s="91">
+        <v>4</v>
+      </c>
       <c r="N13" s="72"/>
       <c r="O13" s="75"/>
       <c r="P13" s="75"/>
       <c r="Q13" s="75"/>
     </row>
     <row r="14" spans="1:17" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="9"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="80">
         <v>2</v>
       </c>
       <c r="D14" s="74">
         <v>3</v>
       </c>
-      <c r="E14" s="74"/>
+      <c r="E14" s="74">
+        <v>2</v>
+      </c>
       <c r="F14" s="74"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="74"/>
-      <c r="I14" s="74"/>
+      <c r="G14" s="74">
+        <v>2</v>
+      </c>
+      <c r="H14" s="74">
+        <v>2</v>
+      </c>
+      <c r="I14" s="74">
+        <v>2</v>
+      </c>
       <c r="J14" s="74"/>
-      <c r="K14" s="74"/>
-      <c r="L14" s="74"/>
-      <c r="M14" s="74"/>
+      <c r="K14" s="74">
+        <v>1</v>
+      </c>
+      <c r="L14" s="74">
+        <v>1</v>
+      </c>
+      <c r="M14" s="74">
+        <v>1</v>
+      </c>
       <c r="N14" s="74"/>
       <c r="O14" s="72"/>
-      <c r="P14" s="74"/>
-      <c r="Q14" s="74"/>
+      <c r="P14" s="92"/>
+      <c r="Q14" s="92">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:17" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="10"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="79" t="s">
         <v>34</v>
       </c>
       <c r="D15" s="75"/>
       <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="75"/>
-      <c r="I15" s="75"/>
-      <c r="J15" s="75"/>
+      <c r="F15" s="75">
+        <v>2</v>
+      </c>
+      <c r="G15" s="75">
+        <v>2</v>
+      </c>
+      <c r="H15" s="75">
+        <v>2</v>
+      </c>
+      <c r="I15" s="75">
+        <v>2</v>
+      </c>
+      <c r="J15" s="75">
+        <v>1</v>
+      </c>
       <c r="K15" s="75"/>
       <c r="L15" s="75"/>
       <c r="M15" s="75"/>
       <c r="N15" s="75"/>
-      <c r="O15" s="75"/>
+      <c r="O15" s="92"/>
       <c r="P15" s="72"/>
-      <c r="Q15" s="75"/>
+      <c r="Q15" s="92"/>
     </row>
     <row r="16" spans="1:17" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="9"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="80">
         <v>2</v>
       </c>
       <c r="D16" s="74">
         <v>2</v>
       </c>
-      <c r="E16" s="74"/>
+      <c r="E16" s="74">
+        <v>1</v>
+      </c>
       <c r="F16" s="74"/>
       <c r="G16" s="74"/>
-      <c r="H16" s="74"/>
-      <c r="I16" s="74"/>
-      <c r="J16" s="74"/>
+      <c r="H16" s="74">
+        <v>1</v>
+      </c>
+      <c r="I16" s="74">
+        <v>2</v>
+      </c>
+      <c r="J16" s="74">
+        <v>1</v>
+      </c>
       <c r="K16" s="74"/>
-      <c r="L16" s="74"/>
+      <c r="L16" s="74">
+        <v>1</v>
+      </c>
       <c r="M16" s="74"/>
       <c r="N16" s="74"/>
-      <c r="O16" s="74"/>
-      <c r="P16" s="74"/>
+      <c r="O16" s="92">
+        <v>1</v>
+      </c>
+      <c r="P16" s="92"/>
       <c r="Q16" s="72"/>
     </row>
   </sheetData>

</xml_diff>